<commit_message>
Feature upgrade work in Jupyter Notebook - spreadsheet export functions
</commit_message>
<xml_diff>
--- a/data/Buildings_FNSB.xlsx
+++ b/data/Buildings_FNSB.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\fnsb-benchmark\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5F8E33F9-4531-4091-BFF1-A703387838D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Building" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="299">
   <si>
     <t>Site ID</t>
   </si>
@@ -929,11 +923,17 @@
       <t>make sure "Site ID" header rows starts on Row 3)</t>
     </r>
   </si>
+  <si>
+    <t>BOR</t>
+  </si>
+  <si>
+    <t>SD-Borealis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1338,18 +1338,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L139"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,6 +3862,23 @@
         <v>21</v>
       </c>
     </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>297</v>
+      </c>
+      <c r="B140" t="s">
+        <v>298</v>
+      </c>
+      <c r="C140" t="s">
+        <v>293</v>
+      </c>
+      <c r="H140">
+        <v>0</v>
+      </c>
+      <c r="J140" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>